<commit_message>
st dev was not obvious
</commit_message>
<xml_diff>
--- a/dataAnalysisGraphs.xlsx
+++ b/dataAnalysisGraphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elizabeth Barnes\w19-360420-machine-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003BA11C-16B4-4A19-98A3-1C461A456F06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B45FA10-FE8B-4782-AA99-95453F5000E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="7500" windowHeight="9345" firstSheet="1" activeTab="1" xr2:uid="{4D271E23-BBA0-41FB-8BFF-21670A73DBD9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4D271E23-BBA0-41FB-8BFF-21670A73DBD9}"/>
   </bookViews>
   <sheets>
     <sheet name="properly up to k=52" sheetId="10" r:id="rId1"/>
@@ -191,11 +191,49 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Graph 1: Mean accuracy as a function</a:t>
+              <a:t>Graph 1: variation</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of k</a:t>
+              <a:t> and standard deviation of </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>mean accuracy, precision and recall </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>as a function of K</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -209,26 +247,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -251,27 +269,28 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln>
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
-              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:errBars>
@@ -281,10 +300,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'properly up to k=52'!$C$2:$C$11</c:f>
+                <c:f>'properly up to k=52'!$C$2:$C$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="26"/>
                   <c:pt idx="0">
                     <c:v>1.3035250446163E-4</c:v>
                   </c:pt>
@@ -314,16 +333,64 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>1.43819892920879E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.3896975609756099E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1.4319474122546E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>1.5239500297441999E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.59519428911362E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.53146341463414E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.6993037477691601E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.8307005353955801E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.10305080309339E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>2.11561308744793E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.9690479476501901E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>2.39360761451516E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>2.47326591314692E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>3.0861989292088002E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>3.2196966091612101E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>3.8537915526472001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>5.4559521713265697E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'properly up to k=52'!$C$2:$C$11</c:f>
+                <c:f>'properly up to k=52'!$C$2:$C$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="26"/>
                   <c:pt idx="0">
                     <c:v>1.3035250446163E-4</c:v>
                   </c:pt>
@@ -353,6 +420,461 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>1.43819892920879E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.3896975609756099E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1.4319474122546E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>1.5239500297441999E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.59519428911362E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.53146341463414E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.6993037477691601E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.8307005353955801E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.10305080309339E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>2.11561308744793E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.9690479476501901E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>2.39360761451516E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>2.47326591314692E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>3.0861989292088002E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>3.2196966091612101E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>3.8537915526472001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>5.4559521713265697E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'properly up to k=52'!$A$2:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'properly up to k=52'!$B$2:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.95875121951220799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96958048780489103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96873170731708602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96780000000001298</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96633658536586697</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96542439024391502</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96339024390245198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96175121951220899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96099512195123304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96006341463415901</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95958048780489003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95815121951220705</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95678048780489</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95602926829269297</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95582926829269399</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.95353170731708203</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.95093170731708299</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.94962439024391099</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.94850731707317804</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.94500487804878497</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.94296585365853902</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.94053658536585505</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.93686341463414302</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.932756097560971</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.92916585365853199</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.92185853658535799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B97F-47E1-B63E-0B7ED83EE8B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'properly up to k=52'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>precision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                  <a:alpha val="45000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'properly up to k=52'!$E$2:$E$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="26"/>
+                  <c:pt idx="0">
+                    <c:v>4.7714640785415601E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.77556044219195E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.64900734634861E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.2464542904449099E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.26965979328656E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.18650711423927E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.2031422668740201E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.8455309413304401E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.7678878391753502E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.7524199160673098E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.89261652334062E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.2705647225273198E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.7162824273671602E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.4721134161661297E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.3511177342367902E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.5186510884705797E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.2039294921555199E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>3.3033501101852102E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>3.2679150888109698E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>3.0708907033740802E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>3.24224343929803E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>3.0723041099043301E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>3.36962896345218E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>3.3134801038269099E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>3.3462509282225402E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.11641724635315E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'properly up to k=52'!$E$2:$E$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="26"/>
+                  <c:pt idx="0">
+                    <c:v>4.7714640785415601E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.77556044219195E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.64900734634861E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.2464542904449099E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.26965979328656E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.18650711423927E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.2031422668740201E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.8455309413304401E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.7678878391753502E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.7524199160673098E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.89261652334062E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.2705647225273198E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.7162824273671602E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.4721134161661297E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.3511177342367902E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.5186510884705797E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.2039294921555199E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>3.3033501101852102E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>3.2679150888109698E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>3.0708907033740802E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>3.24224343929803E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>3.0723041099043301E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>3.36962896345218E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>3.3134801038269099E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>3.3462509282225402E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.11641724635315E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -460,87 +982,87 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'properly up to k=52'!$B$2:$B$27</c:f>
+              <c:f>'properly up to k=52'!$D$2:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0.95875121951220799</c:v>
+                  <c:v>0.94979240732366399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96958048780489103</c:v>
+                  <c:v>0.95429381001437996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.96873170731708602</c:v>
+                  <c:v>0.95650083667380303</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96780000000001298</c:v>
+                  <c:v>0.95720081453523298</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96633658536586697</c:v>
+                  <c:v>0.95915359510482401</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.96542439024391502</c:v>
+                  <c:v>0.96173409215292704</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.96339024390245198</c:v>
+                  <c:v>0.96245357285286603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96175121951220899</c:v>
+                  <c:v>0.96300018682145005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.96099512195123304</c:v>
+                  <c:v>0.96397051663980604</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.96006341463415901</c:v>
+                  <c:v>0.96491511078053505</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.95958048780489003</c:v>
+                  <c:v>0.96581465005462797</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.95815121951220705</c:v>
+                  <c:v>0.96616495698367999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.95678048780489</c:v>
+                  <c:v>0.96624516707256003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.95602926829269297</c:v>
+                  <c:v>0.96721273677402098</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.95582926829269399</c:v>
+                  <c:v>0.96870301718311502</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.95353170731708203</c:v>
+                  <c:v>0.96896798722742705</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.95093170731708299</c:v>
+                  <c:v>0.96967939696192096</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.94962439024391099</c:v>
+                  <c:v>0.97027680776743397</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.94850731707317804</c:v>
+                  <c:v>0.97137652981700995</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.94500487804878497</c:v>
+                  <c:v>0.97096397977518001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.94296585365853902</c:v>
+                  <c:v>0.97107131106723699</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.94053658536585505</c:v>
+                  <c:v>0.97298745818115495</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.93686341463414302</c:v>
+                  <c:v>0.972961521477957</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.932756097560971</c:v>
+                  <c:v>0.97442756077429904</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.92916585365853199</c:v>
+                  <c:v>0.97621022799767099</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.92185853658535799</c:v>
+                  <c:v>0.97834372799258695</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -548,7 +1070,425 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B97F-47E1-B63E-0B7ED83EE8B7}"/>
+              <c16:uniqueId val="{00000007-B97F-47E1-B63E-0B7ED83EE8B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'properly up to k=52'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'properly up to k=52'!$G$2:$G$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="26"/>
+                  <c:pt idx="0">
+                    <c:v>8.6612233445681596E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.4846138328652104E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.6291106302021803E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.6501040233551696E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.4726772663844703E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.5862753701010895E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.8831671064697995E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.2475475884885401E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>8.8433673762411196E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>8.5929625063622603E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>8.8435368392079201E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>8.5370332934253505E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.4519809621254603E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.01607080765902E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.0471388056820499E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.0914986634355101E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.2062828386201201E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.38238532103768E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.3530976840233401E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.3530864574767599E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1.53902934008175E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>1.6457531355913201E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>1.9705936956333999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.2615228110943E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>2.6509786452511498E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.8108529716865702E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'properly up to k=52'!$G$2:$G$27</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="26"/>
+                  <c:pt idx="0">
+                    <c:v>8.6612233445681596E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.4846138328652104E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.6291106302021803E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.6501040233551696E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.4726772663844703E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.5862753701010895E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.8831671064697995E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.2475475884885401E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>8.8433673762411196E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>8.5929625063622603E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>8.8435368392079201E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>8.5370332934253505E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.4519809621254603E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.01607080765902E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.0471388056820499E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.0914986634355101E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.2062828386201201E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.38238532103768E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.3530976840233401E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.3530864574767599E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1.53902934008175E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>1.6457531355913201E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>1.9705936956333999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.2615228110943E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>2.6509786452511498E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.8108529716865702E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'properly up to k=52'!$A$2:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'properly up to k=52'!$F$2:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0.93142648166690201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95875266396594505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95377949860506295</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94973985260096805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94355276068148097</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93833497885882</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93180264649436195</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92590950351738199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92228716750656903</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.91913074392511696</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.91628643033724</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.91174793044306202</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.90732303833877304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.90441365288702003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.90199424684040697</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.89504895479301605</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.88724496327944802</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.88317435787161402</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.87774887770935694</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.86793139900428495</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.86201138941676703</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.85347729441597098</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.84336603594521697</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.82954570558014795</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.81680068227382896</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.79443368322186902</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B97F-47E1-B63E-0B7ED83EE8B7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -605,8 +1545,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>k nearest neighbours</a:t>
+                  <a:t>k</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> nearest neighbours</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -618,26 +1563,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -684,6 +1609,8 @@
         <c:axId val="442862648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.98"/>
+          <c:min val="0.79"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -722,11 +1649,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>mean</a:t>
+                  <a:t>mean value</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-CA" baseline="0"/>
-                  <a:t> accuracy over 1000 repetitions</a:t>
+                  <a:t> over 1000 repetitions</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-CA"/>
               </a:p>
@@ -740,26 +1667,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -802,13 +1709,6 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
@@ -843,30 +1743,9 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -6715,10 +7594,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'properly up to k=52'!$G$2:$G$11</c:f>
+                <c:f>'properly up to k=52'!$G$2:$G$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="26"/>
                   <c:pt idx="0">
                     <c:v>8.6612233445681596E-4</c:v>
                   </c:pt>
@@ -6748,16 +7627,64 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>8.5929625063622603E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>8.8435368392079201E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>8.5370332934253505E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.4519809621254603E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.01607080765902E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.0471388056820499E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.0914986634355101E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.2062828386201201E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.38238532103768E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.3530976840233401E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.3530864574767599E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1.53902934008175E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>1.6457531355913201E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>1.9705936956333999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.2615228110943E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>2.6509786452511498E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.8108529716865702E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'properly up to k=52'!$G$2:$G$11</c:f>
+                <c:f>'properly up to k=52'!$G$2:$G$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="26"/>
                   <c:pt idx="0">
                     <c:v>8.6612233445681596E-4</c:v>
                   </c:pt>
@@ -6787,6 +7714,54 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>8.5929625063622603E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>8.8435368392079201E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>8.5370332934253505E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>9.4519809621254603E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.01607080765902E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.0471388056820499E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.0914986634355101E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.2062828386201201E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.38238532103768E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.3530976840233401E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.3530864574767599E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1.53902934008175E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>1.6457531355913201E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>1.9705936956333999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.2615228110943E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>2.6509786452511498E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.8108529716865702E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -7449,10 +8424,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'properly up to k=52'!$E$2:$E$11</c:f>
+                <c:f>'properly up to k=52'!$E$2:$E$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="26"/>
                   <c:pt idx="0">
                     <c:v>4.7714640785415601E-4</c:v>
                   </c:pt>
@@ -7482,16 +8457,64 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>3.7524199160673098E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.89261652334062E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.2705647225273198E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.7162824273671602E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.4721134161661297E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.3511177342367902E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.5186510884705797E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.2039294921555199E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>3.3033501101852102E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>3.2679150888109698E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>3.0708907033740802E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>3.24224343929803E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>3.0723041099043301E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>3.36962896345218E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>3.3134801038269099E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>3.3462509282225402E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.11641724635315E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'properly up to k=52'!$E$2:$E$11</c:f>
+                <c:f>'properly up to k=52'!$E$2:$E$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="26"/>
                   <c:pt idx="0">
                     <c:v>4.7714640785415601E-4</c:v>
                   </c:pt>
@@ -7521,6 +8544,54 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>3.7524199160673098E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.89261652334062E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.2705647225273198E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.7162824273671602E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.4721134161661297E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.3511177342367902E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.5186510884705797E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.2039294921555199E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>3.3033501101852102E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>3.2679150888109698E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>3.0708907033740802E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>3.24224343929803E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>3.0723041099043301E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>3.36962896345218E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>3.3134801038269099E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>3.3462509282225402E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.11641724635315E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -12210,46 +13281,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17214,7 +18245,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -17730,7 +18761,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18246,7 +19277,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18762,7 +19793,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19278,7 +20309,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19794,7 +20825,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -20310,7 +21341,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -20826,7 +21857,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -21342,536 +22373,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>591140</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>26829</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114890</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>145892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>557866</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>81616</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>167956</xdr:rowOff>
+      <xdr:rowOff>101810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22869,8 +23384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295EAD86-759A-4D89-A044-AA6C5234C7DF}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="K3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23557,8 +24072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADDBDB0-5F9B-4732-95DA-3795AD9118BC}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="72" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="E1" zoomScale="72" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>